<commit_message>
replace vars in header & footer
</commit_message>
<xml_diff>
--- a/tests/test_singlepage.xlsx
+++ b/tests/test_singlepage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcel/development/phpspreadsheet-template-tool/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361EC579-4848-3540-BC48-446C5887AB12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC74FC-7B0E-B14E-91EF-2CB50AA341F4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="22460" xr2:uid="{C4A62566-9300-AD49-9C40-32B06C18FCDF}"/>
   </bookViews>
@@ -946,8 +946,9 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;CLeistungsübersicht Entlastungsbetrag 2018
+    <oddHeader xml:space="preserve">&amp;CLeistungsübersicht &amp;"-,Fett"Entlastungsbetrag&amp;"-,Standard" &amp;"-,Kursiv"§§jahr§§&amp;"-,Standard"
 </oddHeader>
+    <oddFooter>&amp;LStand &amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replace vars in header & footer (#4)
</commit_message>
<xml_diff>
--- a/tests/test_singlepage.xlsx
+++ b/tests/test_singlepage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcel/development/phpspreadsheet-template-tool/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361EC579-4848-3540-BC48-446C5887AB12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC74FC-7B0E-B14E-91EF-2CB50AA341F4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="22460" xr2:uid="{C4A62566-9300-AD49-9C40-32B06C18FCDF}"/>
   </bookViews>
@@ -946,8 +946,9 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;CLeistungsübersicht Entlastungsbetrag 2018
+    <oddHeader xml:space="preserve">&amp;CLeistungsübersicht &amp;"-,Fett"Entlastungsbetrag&amp;"-,Standard" &amp;"-,Kursiv"§§jahr§§&amp;"-,Standard"
 </oddHeader>
+    <oddFooter>&amp;LStand &amp;D</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>